<commit_message>
excel_import_path : finalise function + examples files update
</commit_message>
<xml_diff>
--- a/inst/extdata/impexp.xlsx
+++ b/inst/extdata/impexp.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="importr1" sheetId="1" r:id="rId1"/>
+    <sheet name="impexp1" sheetId="1" r:id="rId1"/>
     <sheet name="Onglet 2" sheetId="2" r:id="rId2"/>
     <sheet name="Autre onglet 1" sheetId="3" r:id="rId3"/>
     <sheet name="Autre onglet 2" sheetId="4" r:id="rId4"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,6 +87,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -135,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -170,7 +173,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -381,7 +384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -431,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>